<commit_message>
Update student data Excel file
Replaced PD/Student Data.xlsx with a new version. The updated file contains modified student data.
</commit_message>
<xml_diff>
--- a/PD/Student Data.xlsx
+++ b/PD/Student Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -41,243 +41,162 @@
     <t>SAIRA MATLOOB</t>
   </si>
   <si>
-    <t>3310522******</t>
-  </si>
-  <si>
     <t>10001</t>
   </si>
   <si>
     <t>MOIZ AFTAB</t>
   </si>
   <si>
-    <t>3310227******</t>
-  </si>
-  <si>
     <t>10002</t>
   </si>
   <si>
     <t>SALIHA ASHIQ</t>
   </si>
   <si>
-    <t>3310418******</t>
-  </si>
-  <si>
     <t>10003</t>
   </si>
   <si>
     <t>MUHAMMAD ADEEL HASSAN</t>
   </si>
   <si>
-    <t>3310430******</t>
-  </si>
-  <si>
     <t>10004</t>
   </si>
   <si>
     <t>EMAN FATIMA</t>
   </si>
   <si>
-    <t>3310049******</t>
-  </si>
-  <si>
     <t>10005</t>
   </si>
   <si>
     <t>MUHAMMAD HAROON</t>
   </si>
   <si>
-    <t>3310259******</t>
-  </si>
-  <si>
     <t>10006</t>
   </si>
   <si>
     <t>MUHAMMAD AHMAD</t>
   </si>
   <si>
-    <t>3310266******</t>
-  </si>
-  <si>
     <t>10007</t>
   </si>
   <si>
     <t>AMEER HAMZA</t>
   </si>
   <si>
-    <t>3320261******</t>
-  </si>
-  <si>
     <t>10008</t>
   </si>
   <si>
     <t>AMNA JAVID BHATTI</t>
   </si>
   <si>
-    <t>3550301******</t>
-  </si>
-  <si>
     <t>10009</t>
   </si>
   <si>
     <t>MUHAMMAD HAMZA SHABBIR</t>
   </si>
   <si>
-    <t>3330380******</t>
-  </si>
-  <si>
     <t>10010</t>
   </si>
   <si>
     <t>FURQAN SHABBIR</t>
   </si>
   <si>
-    <t>3650182******</t>
-  </si>
-  <si>
     <t>10011</t>
   </si>
   <si>
     <t>MUHAMMAD TAIMOOR KHAN</t>
   </si>
   <si>
-    <t>3330117******</t>
-  </si>
-  <si>
     <t>10012</t>
   </si>
   <si>
     <t>MUHAMMAD WAQAR</t>
   </si>
   <si>
-    <t>3550105******</t>
-  </si>
-  <si>
     <t>10013</t>
   </si>
   <si>
     <t>MOEEZ UR REHMAN</t>
   </si>
   <si>
-    <t>3310215******</t>
-  </si>
-  <si>
     <t>10014</t>
   </si>
   <si>
     <t>MUHAMMAD UZAIR</t>
   </si>
   <si>
-    <t>3330339******</t>
-  </si>
-  <si>
     <t>10015</t>
   </si>
   <si>
     <t>MUHAMMAD ABDULLAH</t>
   </si>
   <si>
-    <t>3310222******</t>
-  </si>
-  <si>
     <t>10016</t>
   </si>
   <si>
     <t>MARIAM ARSHAD</t>
   </si>
   <si>
-    <t>3310207******</t>
-  </si>
-  <si>
     <t>10017</t>
   </si>
   <si>
     <t>SAMEEN AHSAN</t>
   </si>
   <si>
-    <t>3310566******</t>
-  </si>
-  <si>
     <t>10018</t>
   </si>
   <si>
     <t>IRA NADEEM</t>
   </si>
   <si>
-    <t>3310313******</t>
-  </si>
-  <si>
     <t>10019</t>
   </si>
   <si>
     <t>RUBAB NADEEM</t>
   </si>
   <si>
-    <t>3310507******</t>
-  </si>
-  <si>
     <t>10020</t>
   </si>
   <si>
     <t>MARIAM TEHSEEN</t>
   </si>
   <si>
-    <t>3310233******</t>
-  </si>
-  <si>
     <t>10021</t>
   </si>
   <si>
     <t>DANIA MEHMOOD</t>
   </si>
   <si>
-    <t>3550302******</t>
-  </si>
-  <si>
     <t>10022</t>
   </si>
   <si>
     <t>HAMNA ANEES</t>
   </si>
   <si>
-    <t>3310064******</t>
-  </si>
-  <si>
     <t>10023</t>
   </si>
   <si>
     <t>ZARAKSHAN</t>
   </si>
   <si>
-    <t>3310097******</t>
-  </si>
-  <si>
     <t>10024</t>
   </si>
   <si>
     <t>MALEEHA MUNAWAR</t>
   </si>
   <si>
-    <t>3310276******</t>
-  </si>
-  <si>
     <t>10025</t>
   </si>
   <si>
     <t>PAWAN BATOOL</t>
   </si>
   <si>
-    <t>3320258******</t>
-  </si>
-  <si>
     <t>10026</t>
   </si>
   <si>
     <t>AYESHA RAZA</t>
   </si>
   <si>
-    <t>3320268******</t>
-  </si>
-  <si>
     <t>10027</t>
   </si>
   <si>
@@ -290,96 +209,63 @@
     <t>KASHAF ZAHRA</t>
   </si>
   <si>
-    <t>3320399******</t>
-  </si>
-  <si>
     <t>10029</t>
   </si>
   <si>
     <t>AHMAD MAQSOOD</t>
   </si>
   <si>
-    <t>3650124******</t>
-  </si>
-  <si>
     <t>10030</t>
   </si>
   <si>
     <t>HAFIZ MUHAMMAD ABDULLAH</t>
   </si>
   <si>
-    <t>3310275******</t>
-  </si>
-  <si>
     <t>10031</t>
   </si>
   <si>
     <t>INAAM MUSTAFA</t>
   </si>
   <si>
-    <t>3320506******</t>
-  </si>
-  <si>
     <t>10032</t>
   </si>
   <si>
     <t>KASHAF ANWAR</t>
   </si>
   <si>
-    <t>3310576******</t>
-  </si>
-  <si>
     <t>10033</t>
   </si>
   <si>
-    <t>3310290******</t>
-  </si>
-  <si>
     <t>10034</t>
   </si>
   <si>
     <t>MUHAMMAD ZOHAIB</t>
   </si>
   <si>
-    <t>3310024******</t>
-  </si>
-  <si>
     <t>10035</t>
   </si>
   <si>
     <t>SHEHZAD HASSAN</t>
   </si>
   <si>
-    <t>3310386******</t>
-  </si>
-  <si>
     <t>10036</t>
   </si>
   <si>
     <t>ZAINAB SHAHZAD</t>
   </si>
   <si>
-    <t>4210118******</t>
-  </si>
-  <si>
     <t>10037</t>
   </si>
   <si>
     <t>AHMED ILYAS</t>
   </si>
   <si>
-    <t>4250150******</t>
-  </si>
-  <si>
     <t>10038</t>
   </si>
   <si>
     <t>MEER MUHAMMAD MANSHA</t>
   </si>
   <si>
-    <t>3540450******</t>
-  </si>
-  <si>
     <t>10039</t>
   </si>
   <si>
@@ -392,16 +278,10 @@
     <t>ESHA IRFAN</t>
   </si>
   <si>
-    <t>3310208******</t>
-  </si>
-  <si>
     <t>10041</t>
   </si>
   <si>
     <t>MUHAMMAD HASHIR RAHEEM</t>
-  </si>
-  <si>
-    <t>3310009******</t>
   </si>
   <si>
     <t>10042</t>
@@ -417,9 +297,17 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -888,140 +776,146 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1371,8 +1265,8 @@
   <sheetPr/>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1382,7 +1276,7 @@
     <col min="3" max="3" width="15.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" ht="15.75" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1394,465 +1288,465 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3">
+        <v>3310522</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="3">
+        <v>3310227</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="3">
+        <v>3310418</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="3">
+        <v>3310430</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="3">
+        <v>3310049</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B7" s="3">
+        <v>3310259</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B8" s="3">
+        <v>3310266</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="B9" s="3">
+        <v>3320261</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B10" s="3">
+        <v>3550301</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="3">
+        <v>3330380</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="B12" s="3">
+        <v>3650182</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="B13" s="3">
+        <v>3330117</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B14" s="3">
+        <v>3550105</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+      <c r="B15" s="3">
+        <v>3310215</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="B16" s="3">
+        <v>3330339</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B17" s="3">
+        <v>3310222</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1" t="s">
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
+      <c r="B18" s="3">
+        <v>3310207</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="B19" s="3">
+        <v>3310566</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B20" s="3">
+        <v>3310313</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
+      <c r="B21" s="3">
+        <v>3310507</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="B22" s="3">
+        <v>3310233</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B23" s="3">
+        <v>3550302</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="1" t="s">
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
+      <c r="B24" s="3">
+        <v>3310064</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B25" s="3">
+        <v>3310097</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B26" s="3">
+        <v>3310276</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="1" t="s">
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
+      <c r="B27" s="3">
+        <v>3320258</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B28" s="3">
+        <v>3320268</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B29" s="3">
+        <v>3550301</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="1" t="s">
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
+      <c r="B30" s="3">
+        <v>3320399</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="B31" s="3">
+        <v>3650124</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B32" s="3">
+        <v>3310275</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="1" t="s">
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
+      <c r="B33" s="3">
+        <v>3320506</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="1" t="s">
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="B34" s="3">
+        <v>3310576</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3">
+        <v>3310290</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="1" t="s">
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="B36" s="3">
+        <v>3310024</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B37" s="3">
+        <v>3310386</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="1" t="s">
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1" t="s">
+      <c r="B38" s="3">
+        <v>4210118</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="1" t="s">
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="B39" s="3">
+        <v>4250150</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B40" s="3">
+        <v>3540450</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="1" t="s">
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
+      <c r="B41" s="3">
+        <v>3310049</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="1" t="s">
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="B42" s="3">
+        <v>3310208</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B43" s="3">
+        <v>3310009</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>